<commit_message>
Some pointers/notes we went over in class- should be helpful to complete the assignment
REMEMBER TO SHORT THE ETF YOU CHOOSE IN PROPORTION TO THE  SECTOR ALLOCATION USING THE BETA-RISK FOR EACH SECTOR, NOT THE NET EXPOSURE...

- YOU CAN ALSO GO AN LONG AN INVERSE ETF IF YOU CHOOSE
</commit_message>
<xml_diff>
--- a/Risk Management/Portfolio Construction/Portfolio Construction - Exercise 1.xlsx
+++ b/Risk Management/Portfolio Construction/Portfolio Construction - Exercise 1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>TICKER</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>IN CLASS ASSIGNMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REMEMBER TO SHORT THE ETF YOU CHOOSE IN PROPORTION TO THE </t>
+  </si>
+  <si>
+    <t>SECTOR ALLOCATION</t>
+  </si>
+  <si>
+    <t>YOU CAN ALSO GO AN LONG AN INVERSE ETF IF YOU CHOOSE</t>
   </si>
 </sst>
 </file>
@@ -234,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -278,9 +287,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -294,6 +300,32 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -597,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -611,33 +643,34 @@
     <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="7" max="7" width="3.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="29.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="8" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="1"/>
+    <col min="12" max="12" width="3.7109375" style="1" customWidth="1"/>
     <col min="13" max="13" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" style="31" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:16" s="19" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="H1" s="21" t="s">
+      <c r="B1" s="20"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="H1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-      <c r="M1" s="20" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="23"/>
+      <c r="M1" s="19" t="s">
         <v>27</v>
       </c>
+      <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
@@ -673,7 +706,7 @@
       <c r="M2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="29" t="s">
         <v>0</v>
       </c>
       <c r="O2" s="10" t="s">
@@ -715,7 +748,7 @@
       <c r="M3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="30">
         <v>0</v>
       </c>
       <c r="O3" s="6">
@@ -758,7 +791,7 @@
       <c r="M4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="30">
         <v>0</v>
       </c>
       <c r="O4" s="6">
@@ -801,54 +834,56 @@
       <c r="M5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="30" t="s">
         <v>30</v>
       </c>
       <c r="O5" s="7">
-        <v>1010000</v>
+        <v>-1010000</v>
       </c>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="H6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="30">
+        <v>0</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="19">
+      <c r="B7" s="20"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="26">
         <f>SUM(D3:D5)</f>
         <v>3</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="19">
         <f>SUM(E3:E5)</f>
         <v>1250000</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="19">
         <f>SUM(F3:F5)</f>
         <v>1855000</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="9">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="9">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H7" s="4" t="s">
         <v>10</v>
       </c>
@@ -864,7 +899,7 @@
       <c r="M7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="9">
+      <c r="N7" s="30">
         <v>0</v>
       </c>
       <c r="O7" s="6">
@@ -873,9 +908,6 @@
       <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H8" s="4" t="s">
         <v>11</v>
       </c>
@@ -891,7 +923,7 @@
       <c r="M8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N8" s="9">
+      <c r="N8" s="30">
         <v>0</v>
       </c>
       <c r="O8" s="6">
@@ -900,12 +932,6 @@
       <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="25">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="H9" s="4" t="s">
         <v>13</v>
       </c>
@@ -921,21 +947,21 @@
       <c r="M9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="30" t="s">
         <v>35</v>
       </c>
       <c r="O9" s="7">
-        <v>845000</v>
+        <v>-845000</v>
       </c>
       <c r="P9" s="5"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="25">
-        <v>2</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>32</v>
-      </c>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
       <c r="H10" s="4" t="s">
         <v>14</v>
       </c>
@@ -951,7 +977,7 @@
       <c r="M10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="9">
+      <c r="N10" s="30">
         <v>0</v>
       </c>
       <c r="O10" s="6">
@@ -959,13 +985,13 @@
       </c>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
-        <v>3</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>33</v>
-      </c>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
       <c r="H11" s="4" t="s">
         <v>15</v>
       </c>
@@ -981,7 +1007,7 @@
       <c r="M11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="30">
         <v>0</v>
       </c>
       <c r="O11" s="6">
@@ -990,12 +1016,12 @@
       <c r="P11" s="6"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="25">
-        <v>4</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
       <c r="H12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1011,7 +1037,7 @@
       <c r="M12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="30">
         <v>0</v>
       </c>
       <c r="O12" s="6">
@@ -1020,16 +1046,12 @@
       <c r="P12" s="6"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25">
-        <v>5</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
       <c r="H13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1045,7 +1067,7 @@
       <c r="M13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="30">
         <v>0</v>
       </c>
       <c r="O13" s="6">
@@ -1054,76 +1076,170 @@
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="9"/>
+      <c r="N14" s="30"/>
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="H15" s="4" t="s">
+    <row r="15" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="H15" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="22">
         <f>SUM(I3:I13)</f>
         <v>3</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="34">
         <f>SUM(J3:J13)</f>
         <v>1250000</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="34">
         <f>SUM(K3:K13)</f>
         <v>1855000</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="M15" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="33">
+        <v>2</v>
+      </c>
+      <c r="O15" s="34">
+        <f>SUM(O3:O13)</f>
+        <v>-1855000</v>
+      </c>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+    </row>
+    <row r="17" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="H17" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="25">
+        <f ca="1">TODAY()</f>
+        <v>45021</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="24">
         <v>1</v>
       </c>
-      <c r="O15" s="6">
-        <f>SUM(O3:O13)</f>
-        <v>1855000</v>
-      </c>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="25">
+      <c r="B19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="24">
+        <v>2</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="24">
+        <v>3</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="24">
+        <v>4</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="24">
+        <v>5</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="24"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="24">
         <v>6</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B26" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-    </row>
-    <row r="17" spans="2:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B16:F17"/>
-    <mergeCell ref="B13:F15"/>
+    <mergeCell ref="B26:F27"/>
+    <mergeCell ref="B23:F25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>